<commit_message>
Fixed bug when exporting COVID-19 decoding results
</commit_message>
<xml_diff>
--- a/outputs/COVID-19_Trial-1_Stage-1_duplicate-primary_Decoded_JYI.xlsx
+++ b/outputs/COVID-19_Trial-1_Stage-1_duplicate-primary_Decoded_JYI.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="203">
   <si>
     <t xml:space="preserve">Exp 1 </t>
   </si>
@@ -76,6 +76,384 @@
   </si>
   <si>
     <t>exhaustive</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>15,30,32,33,35,40,</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>6,13,17,20,27,36,</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>2,10,11,13,16,26,28,30,32,33,35,</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>2,3,6,17,20,27,</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>15,30,32,33,35,40,</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>6,13,17,20,27,36,</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>2,10,11,13,16,26,28,30,32,33,35,</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>2,3,6,17,20,27,</t>
   </si>
   <si>
     <t>N</t>
@@ -312,7 +690,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -334,11 +712,39 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -372,6 +778,34 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,7 +1132,7 @@
     <col min="4" max="4" width="13" bestFit="true" customWidth="true"/>
     <col min="6" max="7" width="10.5" bestFit="true" customWidth="true"/>
     <col min="11" max="11" width="8.625" style="7" customWidth="true"/>
-    <col min="12" max="12" width="17.3984375" style="7" customWidth="true"/>
+    <col min="12" max="12" width="11.625" style="7" customWidth="true"/>
     <col min="13" max="13" width="16.125" style="8" customWidth="true"/>
     <col min="14" max="14" width="15.625" style="8" customWidth="true"/>
     <col min="10" max="10" width="27.625" customWidth="true"/>
@@ -777,14 +1211,16 @@
         <v>1</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>39</v>
+        <v>165</v>
       </c>
       <c r="K3" s="11">
+        <v>9.4173707246037045e-14</v>
+      </c>
+      <c r="L3" s="11">
         <v>8.9258961331149136e-14</v>
       </c>
-      <c r="L3" s="11"/>
       <c r="M3" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N3" s="12">
         <v>0</v>
@@ -800,13 +1236,16 @@
         <v>2</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>40</v>
+        <v>166</v>
       </c>
       <c r="K4" s="11">
+        <v>3.2264654476638076e-11</v>
+      </c>
+      <c r="L4" s="7">
         <v>3206.974041700526</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N4" s="8">
         <v>0</v>
@@ -822,14 +1261,16 @@
         <v>3</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="K5" s="11">
+        <v>4.2546290836590554e-14</v>
+      </c>
+      <c r="L5" s="11">
         <v>1.8157064413328045e-14</v>
       </c>
-      <c r="L5" s="11"/>
       <c r="M5" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N5" s="8">
         <v>0</v>
@@ -845,14 +1286,16 @@
         <v>4</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="K6" s="11">
+        <v>4.1406945044041648e-14</v>
+      </c>
+      <c r="L6" s="11">
         <v>3.1128679350544044e-14</v>
       </c>
-      <c r="L6" s="11"/>
       <c r="M6" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N6" s="12">
         <v>0</v>
@@ -866,14 +1309,16 @@
         <v>5</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="K7" s="11">
+        <v>7.2926901896424646e-14</v>
+      </c>
+      <c r="L7" s="11">
         <v>3.2965457599574666e-14</v>
       </c>
-      <c r="L7" s="11"/>
       <c r="M7" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N7" s="12">
         <v>0</v>
@@ -889,14 +1334,16 @@
         <v>6</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="K8" s="11">
+        <v>1.305599692323725e-14</v>
+      </c>
+      <c r="L8" s="11">
         <v>2.1136268119442921e-14</v>
       </c>
-      <c r="L8" s="11"/>
       <c r="M8" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N8" s="8">
         <v>0</v>
@@ -912,14 +1359,16 @@
         <v>7</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="K9" s="11">
+        <v>5.9032841884083928e-14</v>
+      </c>
+      <c r="L9" s="11">
         <v>3.4544535505027535e-14</v>
       </c>
-      <c r="L9" s="11"/>
       <c r="M9" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N9" s="12">
         <v>0</v>
@@ -935,14 +1384,16 @@
         <v>8</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="K10" s="11">
+        <v>6.4165572307396838e-14</v>
+      </c>
+      <c r="L10" s="11">
         <v>8.3226816144648875e-15</v>
       </c>
-      <c r="L10" s="11"/>
       <c r="M10" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N10" s="12">
         <v>0</v>
@@ -956,14 +1407,16 @@
         <v>9</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="K11" s="11">
+        <v>3.4504663478753251e-14</v>
+      </c>
+      <c r="L11" s="11">
         <v>2.0060498220472276e-14</v>
       </c>
-      <c r="L11" s="11"/>
       <c r="M11" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N11" s="12">
         <v>0</v>
@@ -979,13 +1432,16 @@
         <v>10</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>42</v>
+        <v>168</v>
       </c>
       <c r="K12" s="11">
+        <v>4.1561105127542348e-10</v>
+      </c>
+      <c r="L12" s="7">
         <v>2023.3898717282343</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N12" s="12">
         <v>0</v>
@@ -1001,13 +1457,16 @@
         <v>11</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>42</v>
+        <v>168</v>
       </c>
       <c r="K13" s="11">
+        <v>2.4072118696229842e-10</v>
+      </c>
+      <c r="L13" s="7">
         <v>2023.3898712486198</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N13" s="12">
         <v>0</v>
@@ -1023,14 +1482,16 @@
         <v>12</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>43</v>
+        <v>169</v>
       </c>
       <c r="K14" s="11">
+        <v>1.8419176049968871e-13</v>
+      </c>
+      <c r="L14" s="11">
         <v>2.7780561026581333e-14</v>
       </c>
-      <c r="L14" s="11"/>
       <c r="M14" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N14" s="12">
         <v>0</v>
@@ -1044,13 +1505,16 @@
         <v>13</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="K15" s="11">
+        <v>2.7164527243506691e-11</v>
+      </c>
+      <c r="L15" s="7">
         <v>3206.9740418154884</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N15" s="8">
         <v>0</v>
@@ -1066,14 +1530,16 @@
         <v>14</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>45</v>
+        <v>171</v>
       </c>
       <c r="K16" s="11">
+        <v>3.7945976748616551e-14</v>
+      </c>
+      <c r="L16" s="11">
         <v>3.7397720149883349e-14</v>
       </c>
-      <c r="L16" s="11"/>
       <c r="M16" s="12" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="N16" s="12">
         <v>0</v>
@@ -1087,13 +1553,16 @@
         <v>15</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>46</v>
+        <v>172</v>
       </c>
       <c r="K17" s="7">
+        <v>2026470.4152908823</v>
+      </c>
+      <c r="L17" s="7">
         <v>22854507.545250315</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>15</v>
+        <v>141</v>
       </c>
       <c r="N17" s="12">
         <v>6875904.2393167084</v>
@@ -1109,13 +1578,16 @@
         <v>16</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>47</v>
+        <v>173</v>
       </c>
       <c r="K18" s="11">
+        <v>1.1795199676910874e-11</v>
+      </c>
+      <c r="L18" s="7">
         <v>2037.9676903681291</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N18" s="12">
         <v>0</v>
@@ -1133,14 +1605,16 @@
         <v>17</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="K19" s="11">
+        <v>7.1367157619477175e-14</v>
+      </c>
+      <c r="L19" s="11">
         <v>3.8605113398785635e-14</v>
       </c>
-      <c r="L19" s="11"/>
       <c r="M19" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N19" s="8">
         <v>0</v>
@@ -1151,14 +1625,16 @@
         <v>18</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="K20" s="11">
+        <v>2.6179521912087643e-14</v>
+      </c>
+      <c r="L20" s="11">
         <v>6.2799095374826451e-14</v>
       </c>
-      <c r="L20" s="11"/>
       <c r="M20" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N20" s="12">
         <v>0</v>
@@ -1169,14 +1645,16 @@
         <v>19</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="K21" s="11">
+        <v>1.5338799995263429e-13</v>
+      </c>
+      <c r="L21" s="11">
         <v>4.4786077298381523e-14</v>
       </c>
-      <c r="L21" s="11"/>
       <c r="M21" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N21" s="12">
         <v>0</v>
@@ -1187,14 +1665,16 @@
         <v>20</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="K22" s="11">
+        <v>1.2624441207420615e-14</v>
+      </c>
+      <c r="L22" s="11">
         <v>1.7894516996976303e-14</v>
       </c>
-      <c r="L22" s="11"/>
       <c r="M22" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N22" s="8">
         <v>0</v>
@@ -1205,14 +1685,16 @@
         <v>21</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="K23" s="11">
+        <v>1.6140537012471578e-13</v>
+      </c>
+      <c r="L23" s="11">
         <v>2.3379728509626456e-14</v>
       </c>
-      <c r="L23" s="11"/>
       <c r="M23" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N23" s="12">
         <v>0</v>
@@ -1223,14 +1705,16 @@
         <v>22</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="K24" s="11">
+        <v>1.3143616525123715e-14</v>
+      </c>
+      <c r="L24" s="11">
         <v>1.9679329361836044e-14</v>
       </c>
-      <c r="L24" s="11"/>
       <c r="M24" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N24" s="12">
         <v>0</v>
@@ -1241,14 +1725,16 @@
         <v>23</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="K25" s="11">
+        <v>3.9465187928895047e-14</v>
+      </c>
+      <c r="L25" s="11">
         <v>6.4258565451250319e-14</v>
       </c>
-      <c r="L25" s="11"/>
       <c r="M25" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N25" s="12">
         <v>0</v>
@@ -1259,14 +1745,16 @@
         <v>24</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="K26" s="11">
+        <v>6.0194905699276006e-14</v>
+      </c>
+      <c r="L26" s="11">
         <v>3.2564223656482415e-14</v>
       </c>
-      <c r="L26" s="11"/>
       <c r="M26" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N26" s="12">
         <v>0</v>
@@ -1277,14 +1765,16 @@
         <v>25</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="K27" s="11">
+        <v>2.5023946566766558e-14</v>
+      </c>
+      <c r="L27" s="11">
         <v>1.2953662089121209e-14</v>
       </c>
-      <c r="L27" s="11"/>
       <c r="M27" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N27" s="12">
         <v>0</v>
@@ -1295,13 +1785,16 @@
         <v>26</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>49</v>
+        <v>175</v>
       </c>
       <c r="K28" s="11">
+        <v>2.8060793470301851e-11</v>
+      </c>
+      <c r="L28" s="7">
         <v>2023.3898698118999</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N28" s="12">
         <v>0</v>
@@ -1312,14 +1805,16 @@
         <v>27</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="K29" s="11">
+        <v>1.7581190795023534e-13</v>
+      </c>
+      <c r="L29" s="11">
         <v>2.8123382904164142e-14</v>
       </c>
-      <c r="L29" s="11"/>
       <c r="M29" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N29" s="8">
         <v>0</v>
@@ -1330,13 +1825,16 @@
         <v>28</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>51</v>
+        <v>177</v>
       </c>
       <c r="K30" s="11">
+        <v>3.9073649268121219e-11</v>
+      </c>
+      <c r="L30" s="7">
         <v>2037.9676916245335</v>
       </c>
       <c r="M30" s="8" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N30" s="12">
         <v>0</v>
@@ -1347,14 +1845,16 @@
         <v>29</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>52</v>
+        <v>178</v>
       </c>
       <c r="K31" s="11">
+        <v>8.66570511316092e-14</v>
+      </c>
+      <c r="L31" s="11">
         <v>9.5706805855534789e-14</v>
       </c>
-      <c r="L31" s="11"/>
       <c r="M31" s="12" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="N31" s="12">
         <v>0</v>
@@ -1365,13 +1865,16 @@
         <v>30</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>53</v>
+        <v>179</v>
       </c>
       <c r="K32" s="11">
+        <v>1.5409571617838822e-11</v>
+      </c>
+      <c r="L32" s="7">
         <v>2037.9676908369913</v>
       </c>
       <c r="M32" s="12" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
       <c r="N32" s="12">
         <v>0.0073139701969969773</v>
@@ -1382,14 +1885,16 @@
         <v>31</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>54</v>
+        <v>180</v>
       </c>
       <c r="K33" s="11">
+        <v>6.4462066080223776e-14</v>
+      </c>
+      <c r="L33" s="11">
         <v>3.8438048447584414e-14</v>
       </c>
-      <c r="L33" s="11"/>
       <c r="M33" s="12" t="s">
-        <v>18</v>
+        <v>144</v>
       </c>
       <c r="N33" s="12">
         <v>0</v>
@@ -1400,13 +1905,16 @@
         <v>32</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>55</v>
+        <v>181</v>
       </c>
       <c r="K34" s="11">
+        <v>2.0825760909476039e-11</v>
+      </c>
+      <c r="L34" s="7">
         <v>2037.9676915465475</v>
       </c>
       <c r="M34" s="12" t="s">
-        <v>19</v>
+        <v>145</v>
       </c>
       <c r="N34" s="12">
         <v>0.050964814588828844</v>
@@ -1417,13 +1925,16 @@
         <v>33</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>55</v>
+        <v>181</v>
       </c>
       <c r="K35" s="11">
+        <v>1.9238257826656695e-10</v>
+      </c>
+      <c r="L35" s="7">
         <v>3206.9740417773032</v>
       </c>
       <c r="M35" s="8" t="s">
-        <v>19</v>
+        <v>145</v>
       </c>
       <c r="N35" s="12">
         <v>4039.1910201484006</v>
@@ -1434,14 +1945,16 @@
         <v>34</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>56</v>
+        <v>182</v>
       </c>
       <c r="K36" s="11">
+        <v>9.3505977518849553e-14</v>
+      </c>
+      <c r="L36" s="11">
         <v>1.9683902155870978e-14</v>
       </c>
-      <c r="L36" s="11"/>
       <c r="M36" s="12" t="s">
-        <v>20</v>
+        <v>146</v>
       </c>
       <c r="N36" s="12">
         <v>0</v>
@@ -1452,13 +1965,16 @@
         <v>35</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>57</v>
+        <v>183</v>
       </c>
       <c r="K37" s="11">
+        <v>1.3929386819009172e-11</v>
+      </c>
+      <c r="L37" s="7">
         <v>2023.3898715397861</v>
       </c>
       <c r="M37" s="12" t="s">
-        <v>21</v>
+        <v>147</v>
       </c>
       <c r="N37" s="12">
         <v>4447.0520474304622</v>
@@ -1469,14 +1985,16 @@
         <v>36</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>58</v>
+        <v>184</v>
       </c>
       <c r="K38" s="11">
+        <v>2.0536502513882167e-13</v>
+      </c>
+      <c r="L38" s="11">
         <v>4.4120027020709978e-14</v>
       </c>
-      <c r="L38" s="11"/>
       <c r="M38" s="12" t="s">
-        <v>22</v>
+        <v>148</v>
       </c>
       <c r="N38" s="8">
         <v>0</v>
@@ -1487,14 +2005,16 @@
         <v>37</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>58</v>
+        <v>184</v>
       </c>
       <c r="K39" s="11">
+        <v>4.0087356216530257e-14</v>
+      </c>
+      <c r="L39" s="11">
         <v>3.1154699040572686e-14</v>
       </c>
-      <c r="L39" s="11"/>
       <c r="M39" s="12" t="s">
-        <v>22</v>
+        <v>148</v>
       </c>
       <c r="N39" s="12">
         <v>0</v>
@@ -1512,14 +2032,16 @@
         <v>38</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>58</v>
+        <v>184</v>
       </c>
       <c r="K40" s="11">
+        <v>4.7108381823803501e-14</v>
+      </c>
+      <c r="L40" s="11">
         <v>3.3557422003041275e-14</v>
       </c>
-      <c r="L40" s="11"/>
       <c r="M40" s="12" t="s">
-        <v>22</v>
+        <v>148</v>
       </c>
       <c r="N40" s="12">
         <v>0</v>
@@ -1537,14 +2059,16 @@
         <v>39</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>58</v>
+        <v>184</v>
       </c>
       <c r="K41" s="11">
+        <v>6.8376732632088838e-14</v>
+      </c>
+      <c r="L41" s="11">
         <v>1.1686052927975319e-13</v>
       </c>
-      <c r="L41" s="11"/>
       <c r="M41" s="12" t="s">
-        <v>22</v>
+        <v>148</v>
       </c>
       <c r="N41" s="12">
         <v>0</v>
@@ -1562,13 +2086,16 @@
         <v>40</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>59</v>
+        <v>185</v>
       </c>
       <c r="K42" s="11">
+        <v>19079.305893565994</v>
+      </c>
+      <c r="L42" s="7">
         <v>221211.54890111086</v>
       </c>
       <c r="M42" s="8" t="s">
-        <v>23</v>
+        <v>149</v>
       </c>
       <c r="N42" s="12">
         <v>71877.511548159659</v>
@@ -1583,10 +2110,10 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="J43" s="0" t="s">
-        <v>60</v>
+        <v>186</v>
       </c>
       <c r="M43" s="8" t="s">
-        <v>24</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" x14ac:dyDescent="0.3">
@@ -1638,14 +2165,16 @@
         <v>1</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>61</v>
+        <v>187</v>
       </c>
       <c r="K45" s="11">
+        <v>5.9142052345911541e-14</v>
+      </c>
+      <c r="L45" s="11">
         <v>5.5920590535667589e-14</v>
       </c>
-      <c r="L45" s="11"/>
       <c r="M45" s="12" t="s">
-        <v>25</v>
+        <v>151</v>
       </c>
       <c r="N45" s="8">
         <v>0</v>
@@ -1661,13 +2190,16 @@
         <v>2</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>62</v>
+        <v>188</v>
       </c>
       <c r="K46" s="11">
+        <v>1.5709973366889658e-10</v>
+      </c>
+      <c r="L46" s="7">
         <v>8676.7329346712613</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>25</v>
+        <v>151</v>
       </c>
       <c r="N46" s="8">
         <v>0</v>
@@ -1681,13 +2213,16 @@
         <v>3</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>62</v>
+        <v>188</v>
       </c>
       <c r="K47" s="11">
+        <v>2.9654731560669449e-11</v>
+      </c>
+      <c r="L47" s="7">
         <v>7040.5415997287537</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>25</v>
+        <v>151</v>
       </c>
       <c r="N47" s="8">
         <v>0</v>
@@ -1703,14 +2238,16 @@
         <v>4</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>63</v>
+        <v>189</v>
       </c>
       <c r="K48" s="11">
+        <v>5.7955368070565477e-14</v>
+      </c>
+      <c r="L48" s="11">
         <v>7.1400572980406432e-14</v>
       </c>
-      <c r="L48" s="11"/>
       <c r="M48" s="12" t="s">
-        <v>25</v>
+        <v>151</v>
       </c>
       <c r="N48" s="8">
         <v>0</v>
@@ -1726,14 +2263,16 @@
         <v>5</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>63</v>
+        <v>189</v>
       </c>
       <c r="K49" s="11">
+        <v>5.4906989840037703e-14</v>
+      </c>
+      <c r="L49" s="11">
         <v>6.3809017769427716e-14</v>
       </c>
-      <c r="L49" s="11"/>
       <c r="M49" s="12" t="s">
-        <v>25</v>
+        <v>151</v>
       </c>
       <c r="N49" s="8">
         <v>0</v>
@@ -1747,13 +2286,16 @@
         <v>6</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>64</v>
+        <v>190</v>
       </c>
       <c r="K50" s="11">
+        <v>2.4318284855381621e-11</v>
+      </c>
+      <c r="L50" s="7">
         <v>7040.5415997301006</v>
       </c>
       <c r="M50" s="8" t="s">
-        <v>26</v>
+        <v>152</v>
       </c>
       <c r="N50" s="8">
         <v>0.0046357344748151341</v>
@@ -1767,14 +2309,16 @@
         <v>7</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="K51" s="11">
+        <v>6.8126834544653738e-14</v>
+      </c>
+      <c r="L51" s="11">
         <v>5.1568544575775172e-14</v>
       </c>
-      <c r="L51" s="11"/>
       <c r="M51" s="12" t="s">
-        <v>27</v>
+        <v>153</v>
       </c>
       <c r="N51" s="8">
         <v>0</v>
@@ -1790,14 +2334,16 @@
         <v>8</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="K52" s="11">
+        <v>1.5015113393277146e-13</v>
+      </c>
+      <c r="L52" s="11">
         <v>1.5624387688440888e-13</v>
       </c>
-      <c r="L52" s="11"/>
       <c r="M52" s="12" t="s">
-        <v>27</v>
+        <v>153</v>
       </c>
       <c r="N52" s="8">
         <v>0</v>
@@ -1813,14 +2359,16 @@
         <v>9</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="K53" s="11">
+        <v>4.7882451043300727e-14</v>
+      </c>
+      <c r="L53" s="11">
         <v>2.8881150937641972e-14</v>
       </c>
-      <c r="L53" s="11"/>
       <c r="M53" s="12" t="s">
-        <v>27</v>
+        <v>153</v>
       </c>
       <c r="N53" s="8">
         <v>0</v>
@@ -1834,14 +2382,16 @@
         <v>10</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="K54" s="11">
+        <v>4.8106960143178912e-14</v>
+      </c>
+      <c r="L54" s="11">
         <v>5.4736596119394221e-14</v>
       </c>
-      <c r="L54" s="11"/>
       <c r="M54" s="12" t="s">
-        <v>27</v>
+        <v>153</v>
       </c>
       <c r="N54" s="8">
         <v>0</v>
@@ -1857,14 +2407,16 @@
         <v>11</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="K55" s="11">
+        <v>9.5956780693052677e-14</v>
+      </c>
+      <c r="L55" s="11">
         <v>1.0819585776431437e-13</v>
       </c>
-      <c r="L55" s="11"/>
       <c r="M55" s="12" t="s">
-        <v>27</v>
+        <v>153</v>
       </c>
       <c r="N55" s="8">
         <v>0</v>
@@ -1880,14 +2432,16 @@
         <v>12</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="K56" s="11">
+        <v>1.3124068087427173e-13</v>
+      </c>
+      <c r="L56" s="11">
         <v>7.1906830622859601e-14</v>
       </c>
-      <c r="L56" s="11"/>
       <c r="M56" s="12" t="s">
-        <v>27</v>
+        <v>153</v>
       </c>
       <c r="N56" s="8">
         <v>0</v>
@@ -1901,13 +2455,16 @@
         <v>13</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>66</v>
+        <v>192</v>
       </c>
       <c r="K57" s="11">
+        <v>166463.19273881597</v>
+      </c>
+      <c r="L57" s="7">
         <v>1888291.0258768722</v>
       </c>
       <c r="M57" s="8" t="s">
-        <v>28</v>
+        <v>154</v>
       </c>
       <c r="N57" s="8">
         <v>569745.42726842279</v>
@@ -1923,14 +2480,16 @@
         <v>14</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="K58" s="11">
+        <v>8.1071353671342344e-14</v>
+      </c>
+      <c r="L58" s="11">
         <v>1.0076960784890403e-13</v>
       </c>
-      <c r="L58" s="11"/>
       <c r="M58" s="12" t="s">
-        <v>29</v>
+        <v>155</v>
       </c>
       <c r="N58" s="8">
         <v>0</v>
@@ -1946,14 +2505,16 @@
         <v>15</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="K59" s="11">
+        <v>7.3091880252498255e-14</v>
+      </c>
+      <c r="L59" s="11">
         <v>7.5078374789524126e-14</v>
       </c>
-      <c r="L59" s="11"/>
       <c r="M59" s="12" t="s">
-        <v>29</v>
+        <v>155</v>
       </c>
       <c r="N59" s="8">
         <v>0</v>
@@ -1969,14 +2530,16 @@
         <v>16</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="K60" s="11">
+        <v>9.1011253511929735e-14</v>
+      </c>
+      <c r="L60" s="11">
         <v>9.2974766241514898e-14</v>
       </c>
-      <c r="L60" s="11"/>
       <c r="M60" s="12" t="s">
-        <v>29</v>
+        <v>155</v>
       </c>
       <c r="N60" s="8">
         <v>0</v>
@@ -1994,13 +2557,16 @@
         <v>17</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>68</v>
+        <v>194</v>
       </c>
       <c r="K61" s="11">
+        <v>3.4587599828891116e-10</v>
+      </c>
+      <c r="L61" s="7">
         <v>130663.00733827474</v>
       </c>
       <c r="M61" s="8" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="N61" s="8">
         <v>4625.4189173007389</v>
@@ -2018,14 +2584,16 @@
         <v>18</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>69</v>
+        <v>195</v>
       </c>
       <c r="K62" s="11">
+        <v>8.1286729747138925e-14</v>
+      </c>
+      <c r="L62" s="11">
         <v>6.1084744588894114e-14</v>
       </c>
-      <c r="L62" s="11"/>
       <c r="M62" s="12" t="s">
-        <v>31</v>
+        <v>157</v>
       </c>
       <c r="N62" s="8">
         <v>0</v>
@@ -2043,14 +2611,16 @@
         <v>19</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>69</v>
+        <v>195</v>
       </c>
       <c r="K63" s="11">
+        <v>1.9030371441315751e-13</v>
+      </c>
+      <c r="L63" s="11">
         <v>2.8589339635288752e-13</v>
       </c>
-      <c r="L63" s="11"/>
       <c r="M63" s="12" t="s">
-        <v>31</v>
+        <v>157</v>
       </c>
       <c r="N63" s="8">
         <v>0</v>
@@ -2068,13 +2638,16 @@
         <v>20</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
       <c r="K64" s="11">
+        <v>6.4888033099355141e-10</v>
+      </c>
+      <c r="L64" s="7">
         <v>7040.5415997098398</v>
       </c>
       <c r="M64" s="8" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
       <c r="N64" s="12">
         <v>34968.420008593705</v>
@@ -2092,14 +2665,16 @@
         <v>21</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>71</v>
+        <v>197</v>
       </c>
       <c r="K65" s="11">
+        <v>5.112538765008569e-14</v>
+      </c>
+      <c r="L65" s="11">
         <v>5.9429748557725619e-14</v>
       </c>
-      <c r="L65" s="11"/>
       <c r="M65" s="12" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="N65" s="8">
         <v>0</v>
@@ -2117,14 +2692,16 @@
         <v>22</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>71</v>
+        <v>197</v>
       </c>
       <c r="K66" s="11">
+        <v>1.8790961524412153e-13</v>
+      </c>
+      <c r="L66" s="11">
         <v>2.2406935396954661e-13</v>
       </c>
-      <c r="L66" s="11"/>
       <c r="M66" s="12" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="N66" s="8">
         <v>0</v>
@@ -2142,14 +2719,16 @@
         <v>23</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>71</v>
+        <v>197</v>
       </c>
       <c r="K67" s="11">
+        <v>8.3873145050286647e-14</v>
+      </c>
+      <c r="L67" s="11">
         <v>9.6166151934703541e-14</v>
       </c>
-      <c r="L67" s="11"/>
       <c r="M67" s="12" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="N67" s="8">
         <v>0</v>
@@ -2167,14 +2746,16 @@
         <v>24</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>71</v>
+        <v>197</v>
       </c>
       <c r="K68" s="11">
+        <v>1.5223024287171512e-13</v>
+      </c>
+      <c r="L68" s="11">
         <v>1.2318640148928734e-13</v>
       </c>
-      <c r="L68" s="11"/>
       <c r="M68" s="12" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="N68" s="8">
         <v>0</v>
@@ -2192,14 +2773,16 @@
         <v>25</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>71</v>
+        <v>197</v>
       </c>
       <c r="K69" s="11">
+        <v>6.9189486513191238e-14</v>
+      </c>
+      <c r="L69" s="11">
         <v>3.5087278777198338e-14</v>
       </c>
-      <c r="L69" s="11"/>
       <c r="M69" s="12" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="N69" s="8">
         <v>0</v>
@@ -2217,14 +2800,16 @@
         <v>26</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>71</v>
+        <v>197</v>
       </c>
       <c r="K70" s="11">
+        <v>1.4677422287110146e-13</v>
+      </c>
+      <c r="L70" s="11">
         <v>1.703963200535846e-13</v>
       </c>
-      <c r="L70" s="11"/>
       <c r="M70" s="12" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="N70" s="8">
         <v>0</v>
@@ -2242,13 +2827,16 @@
         <v>27</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>72</v>
+        <v>198</v>
       </c>
       <c r="K71" s="11">
+        <v>2.174537901639857e-10</v>
+      </c>
+      <c r="L71" s="7">
         <v>130663.00733828441</v>
       </c>
       <c r="M71" s="8" t="s">
-        <v>34</v>
+        <v>160</v>
       </c>
       <c r="N71" s="8">
         <v>0.00050699800822514435</v>
@@ -2266,14 +2854,16 @@
         <v>28</v>
       </c>
       <c r="J72" s="0" t="s">
-        <v>73</v>
+        <v>199</v>
       </c>
       <c r="K72" s="11">
+        <v>9.3232164205595768e-14</v>
+      </c>
+      <c r="L72" s="11">
         <v>1.2822322029643258e-13</v>
       </c>
-      <c r="L72" s="11"/>
       <c r="M72" s="12" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="N72" s="8">
         <v>0</v>
@@ -2291,14 +2881,16 @@
         <v>29</v>
       </c>
       <c r="J73" s="0" t="s">
-        <v>73</v>
+        <v>199</v>
       </c>
       <c r="K73" s="11">
+        <v>1.4047294356371754e-13</v>
+      </c>
+      <c r="L73" s="11">
         <v>2.2360001072584933e-13</v>
       </c>
-      <c r="L73" s="11"/>
       <c r="M73" s="12" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="N73" s="8">
         <v>0</v>
@@ -2316,14 +2908,16 @@
         <v>30</v>
       </c>
       <c r="J74" s="0" t="s">
-        <v>73</v>
+        <v>199</v>
       </c>
       <c r="K74" s="11">
+        <v>8.6646121724411853e-14</v>
+      </c>
+      <c r="L74" s="11">
         <v>9.6823882862188953e-14</v>
       </c>
-      <c r="L74" s="11"/>
       <c r="M74" s="12" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="N74" s="8">
         <v>0</v>
@@ -2341,14 +2935,16 @@
         <v>31</v>
       </c>
       <c r="J75" s="0" t="s">
-        <v>73</v>
+        <v>199</v>
       </c>
       <c r="K75" s="11">
+        <v>1.3583213859481338e-13</v>
+      </c>
+      <c r="L75" s="11">
         <v>1.3450590408979467e-13</v>
       </c>
-      <c r="L75" s="11"/>
       <c r="M75" s="12" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="N75" s="8">
         <v>0</v>
@@ -2366,14 +2962,16 @@
         <v>32</v>
       </c>
       <c r="J76" s="0" t="s">
-        <v>73</v>
+        <v>199</v>
       </c>
       <c r="K76" s="11">
+        <v>9.1252491312543966e-14</v>
+      </c>
+      <c r="L76" s="11">
         <v>1.2329728651362639e-13</v>
       </c>
-      <c r="L76" s="11"/>
       <c r="M76" s="12" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="N76" s="8">
         <v>0</v>
@@ -2391,14 +2989,16 @@
         <v>33</v>
       </c>
       <c r="J77" s="0" t="s">
-        <v>73</v>
+        <v>199</v>
       </c>
       <c r="K77" s="11">
+        <v>1.0873273321605347e-13</v>
+      </c>
+      <c r="L77" s="11">
         <v>5.452262125818383e-14</v>
       </c>
-      <c r="L77" s="11"/>
       <c r="M77" s="12" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="N77" s="8">
         <v>0</v>
@@ -2416,14 +3016,16 @@
         <v>34</v>
       </c>
       <c r="J78" s="0" t="s">
-        <v>73</v>
+        <v>199</v>
       </c>
       <c r="K78" s="11">
+        <v>1.1555979987034171e-13</v>
+      </c>
+      <c r="L78" s="11">
         <v>7.5357654340201377e-14</v>
       </c>
-      <c r="L78" s="11"/>
       <c r="M78" s="12" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="N78" s="8">
         <v>0</v>
@@ -2441,14 +3043,16 @@
         <v>35</v>
       </c>
       <c r="J79" s="0" t="s">
-        <v>73</v>
+        <v>199</v>
       </c>
       <c r="K79" s="11">
+        <v>8.1338640343460776e-14</v>
+      </c>
+      <c r="L79" s="11">
         <v>5.4833016050723874e-14</v>
       </c>
-      <c r="L79" s="11"/>
       <c r="M79" s="12" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="N79" s="8">
         <v>0</v>
@@ -2466,13 +3070,16 @@
         <v>36</v>
       </c>
       <c r="J80" s="0" t="s">
-        <v>74</v>
+        <v>200</v>
       </c>
       <c r="K80" s="11">
+        <v>76113.358698137381</v>
+      </c>
+      <c r="L80" s="7">
         <v>2115839.9462884348</v>
       </c>
       <c r="M80" s="8" t="s">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="N80" s="8">
         <v>554084.67939013476</v>
@@ -2490,14 +3097,16 @@
         <v>37</v>
       </c>
       <c r="J81" s="0" t="s">
-        <v>75</v>
+        <v>201</v>
       </c>
       <c r="K81" s="11">
+        <v>8.2100115967578173e-14</v>
+      </c>
+      <c r="L81" s="11">
         <v>9.5097945412455815e-14</v>
       </c>
-      <c r="L81" s="11"/>
       <c r="M81" s="12" t="s">
-        <v>37</v>
+        <v>163</v>
       </c>
       <c r="N81" s="8">
         <v>0</v>
@@ -2515,14 +3124,16 @@
         <v>38</v>
       </c>
       <c r="J82" s="0" t="s">
-        <v>75</v>
+        <v>201</v>
       </c>
       <c r="K82" s="11">
+        <v>7.8491305662686163e-14</v>
+      </c>
+      <c r="L82" s="11">
         <v>4.491646286203869e-14</v>
       </c>
-      <c r="L82" s="11"/>
       <c r="M82" s="12" t="s">
-        <v>37</v>
+        <v>163</v>
       </c>
       <c r="N82" s="8">
         <v>0</v>
@@ -2540,14 +3151,16 @@
         <v>39</v>
       </c>
       <c r="J83" s="0" t="s">
-        <v>75</v>
+        <v>201</v>
       </c>
       <c r="K83" s="11">
+        <v>5.2444641095643635e-14</v>
+      </c>
+      <c r="L83" s="11">
         <v>6.551454150245555e-14</v>
       </c>
-      <c r="L83" s="11"/>
       <c r="M83" s="12" t="s">
-        <v>37</v>
+        <v>163</v>
       </c>
       <c r="N83" s="8">
         <v>0</v>
@@ -2565,14 +3178,16 @@
         <v>40</v>
       </c>
       <c r="J84" s="0" t="s">
-        <v>75</v>
+        <v>201</v>
       </c>
       <c r="K84" s="11">
+        <v>9.4430179530853262e-14</v>
+      </c>
+      <c r="L84" s="11">
         <v>5.6755011461901863e-14</v>
       </c>
-      <c r="L84" s="11"/>
       <c r="M84" s="12" t="s">
-        <v>37</v>
+        <v>163</v>
       </c>
       <c r="N84" s="8">
         <v>0</v>
@@ -2587,10 +3202,10 @@
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="J85" s="0" t="s">
-        <v>76</v>
+        <v>202</v>
       </c>
       <c r="M85" s="8" t="s">
-        <v>38</v>
+        <v>164</v>
       </c>
     </row>
     <row r="86" x14ac:dyDescent="0.3">

</xml_diff>